<commit_message>
Remove stray 0 in one of the columns.
</commit_message>
<xml_diff>
--- a/test_images/backup.template_linux.xlsx
+++ b/test_images/backup.template_linux.xlsx
@@ -229,29 +229,29 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:V4"/>
+  <dimension ref="A1:R4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S1" activeCellId="0" sqref="S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.1740890688259"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.246963562753"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.995951417004"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.3157894736842"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.9230769230769"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="26.1376518218623"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="27.4210526315789"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.1012145748988"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="18.5303643724696"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="25.9230769230769"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.1012145748988"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.5303643724696"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.1376518218623"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="26.3522267206478"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="27.6356275303644"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.2105263157895"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="18.6396761133603"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="26.0283400809717"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="6.10526315789474"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="28.3279352226721"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.1052631578947"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="14.5668016194332"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="17.995951417004"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="28.4939271255061"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.2105263157895"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="14.6761133603239"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="18.1012145748988"/>
     <col collapsed="false" hidden="false" max="17" min="17" style="0" width="13.8178137651822"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="8.57085020242915"/>
@@ -440,9 +440,6 @@
       </c>
       <c r="R4" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="V4" s="0" t="n">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>